<commit_message>
Adds studios to Contacts page. Plus reformatting
</commit_message>
<xml_diff>
--- a/AvlZen/App_Data/AvlZen.xlsx
+++ b/AvlZen/App_Data/AvlZen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Places" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="AvlHapBod" sheetId="11" r:id="rId11"/>
     <sheet name="YmcaWdfn" sheetId="13" r:id="rId12"/>
     <sheet name="YmcaReut" sheetId="14" r:id="rId13"/>
+    <sheet name="NrshLifeCtr" sheetId="15" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_cid31" localSheetId="10">AvlHapBod!$J$3</definedName>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="460">
   <si>
     <t>Code</t>
   </si>
@@ -1402,6 +1403,36 @@
   </si>
   <si>
     <t>Lynn</t>
+  </si>
+  <si>
+    <t>NrshLifeCtr</t>
+  </si>
+  <si>
+    <t>Nourishing Life Center of Health</t>
+  </si>
+  <si>
+    <t>http://nourishinglife.com/yoga</t>
+  </si>
+  <si>
+    <t>Dao Flow All - Levels 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>Self Practice (sub)</t>
+  </si>
+  <si>
+    <t>Margaret Kirschner</t>
+  </si>
+  <si>
+    <t>Dao Flow Yoga for Women Level 1</t>
+  </si>
+  <si>
+    <t>Dr. Robin Saraswati</t>
+  </si>
+  <si>
+    <t>Dao Flow Yoga for Women Levels 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>Dao Flow Yoga for Women Level 2</t>
   </si>
 </sst>
 </file>
@@ -1967,10 +1998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2123,6 +2154,17 @@
         <v>438</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>450</v>
+      </c>
+      <c r="B14" t="s">
+        <v>451</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>452</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -2131,9 +2173,10 @@
     <hyperlink ref="C8" r:id="rId3"/>
     <hyperlink ref="C12" r:id="rId4"/>
     <hyperlink ref="C13" r:id="rId5"/>
+    <hyperlink ref="C14" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -3069,7 +3112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -3333,6 +3376,145 @@
       </c>
       <c r="E21" t="s">
         <v>442</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="D2" t="s">
+        <v>453</v>
+      </c>
+      <c r="E2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.4375</v>
+      </c>
+      <c r="D4" t="s">
+        <v>403</v>
+      </c>
+      <c r="E4" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D6" t="s">
+        <v>456</v>
+      </c>
+      <c r="E6" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.4375</v>
+      </c>
+      <c r="D8" t="s">
+        <v>458</v>
+      </c>
+      <c r="E8" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="D9" t="s">
+        <v>453</v>
+      </c>
+      <c r="E9" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D11" t="s">
+        <v>459</v>
+      </c>
+      <c r="E11" t="s">
+        <v>454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oops - Donation Studio Screw up
</commit_message>
<xml_diff>
--- a/AvlZen/App_Data/AvlZen.xlsx
+++ b/AvlZen/App_Data/AvlZen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11430" yWindow="-15" windowWidth="11655" windowHeight="12060" tabRatio="907" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="7440" yWindow="-15" windowWidth="15645" windowHeight="12060" tabRatio="907" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Places" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="472">
   <si>
     <t>Code</t>
   </si>
@@ -787,9 +787,6 @@
     <t>Gentle Flow (Level 1 &amp; 2)</t>
   </si>
   <si>
-    <t>Guided Meditation (All Levels)</t>
-  </si>
-  <si>
     <t>Warm Vinyasa Flow (Level 1 &amp; 2)</t>
   </si>
   <si>
@@ -1168,9 +1165,6 @@
     <t>Yin Yoga (All levels - Beginners Welcome)</t>
   </si>
   <si>
-    <t xml:space="preserve">NO MARCH SCHEDULE UP </t>
-  </si>
-  <si>
     <t>MARCH SCHEDULE NOT UPDATED</t>
   </si>
   <si>
@@ -1300,9 +1294,6 @@
     <t>Lisa Sherman</t>
   </si>
   <si>
-    <t>Cultivating a Meditation Practice (Beginners Welcome)</t>
-  </si>
-  <si>
     <t>Sarah</t>
   </si>
   <si>
@@ -1325,6 +1316,159 @@
   </si>
   <si>
     <t>Yoga Sangha (Level 1 &amp; 2)</t>
+  </si>
+  <si>
+    <t>HOT Bhakti Vinyasa, Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>HOT Flow, Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Slow Flow &amp; Yin, Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Family Yoga, All Levels</t>
+  </si>
+  <si>
+    <t>Slow Flow, Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Yoga &amp; Body Rolling, All Levels</t>
+  </si>
+  <si>
+    <t>Paige</t>
+  </si>
+  <si>
+    <t>Warm Jivamukti, Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Vibrant Breath Yoga, All Levels</t>
+  </si>
+  <si>
+    <t>Beginners’ Yoga, Level 1</t>
+  </si>
+  <si>
+    <t>Kundalini Yoga, All Levels</t>
+  </si>
+  <si>
+    <t>Krystal</t>
+  </si>
+  <si>
+    <t>HOT Flow, Level 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>Tantra Vinyasa, Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Mindful Alignment, Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Yoga Nidra, All Levels</t>
+  </si>
+  <si>
+    <t>Slow Flow &amp; Deep Stretch Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Alex Moody</t>
+  </si>
+  <si>
+    <t>Jane-Anne Tager</t>
+  </si>
+  <si>
+    <t>Tim Burgin</t>
+  </si>
+  <si>
+    <t>Vinyasa Flow All Levels</t>
+  </si>
+  <si>
+    <t>Julia Albertson</t>
+  </si>
+  <si>
+    <t>Deep Core Align &amp; Flow Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Gayle Jann</t>
+  </si>
+  <si>
+    <t>Warm Jivamukti Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Adam Shirley</t>
+  </si>
+  <si>
+    <t>Yoga for Women Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>HOT Align &amp; Flow Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Adam Taylor</t>
+  </si>
+  <si>
+    <t>Nicole Killeen</t>
+  </si>
+  <si>
+    <t>Intuitive Yoga for Beginners Level 1</t>
+  </si>
+  <si>
+    <t>Brian Winslett</t>
+  </si>
+  <si>
+    <t>Restorative &amp; Yin, plus Live Music, All Levels</t>
+  </si>
+  <si>
+    <t>Rebecca Odom</t>
+  </si>
+  <si>
+    <t>Prenatal Yoga &amp; Meditation All Levels</t>
+  </si>
+  <si>
+    <t>Danielle Marie Goldstein</t>
+  </si>
+  <si>
+    <t>Innercise Yoga Flow, Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Kelsey Armbruster</t>
+  </si>
+  <si>
+    <t>Corey Brown</t>
+  </si>
+  <si>
+    <t>Ann-Lee Waite</t>
+  </si>
+  <si>
+    <t>Tanya Naplioueva</t>
+  </si>
+  <si>
+    <t>Gentle &amp; Restorative All Levels</t>
+  </si>
+  <si>
+    <t>Therapeutic Flow All Levels</t>
+  </si>
+  <si>
+    <t>Evan Hart Marsh</t>
+  </si>
+  <si>
+    <t>Natalie Epstein</t>
+  </si>
+  <si>
+    <t>Slow Flow &amp; Yin Level 1</t>
+  </si>
+  <si>
+    <t>Warm Kripalu Flow Level 1&amp;2</t>
+  </si>
+  <si>
+    <t>Meditation in Motion</t>
+  </si>
+  <si>
+    <t>Andrea Rich</t>
+  </si>
+  <si>
+    <t>Janelle Railey</t>
+  </si>
+  <si>
+    <t>Jackie Dobrinska</t>
   </si>
 </sst>
 </file>
@@ -1538,7 +1682,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1620,6 +1764,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1948,7 +2098,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1959,24 +2109,24 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" t="s">
         <v>264</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>265</v>
       </c>
-      <c r="C3" t="s">
-        <v>266</v>
-      </c>
       <c r="D3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1987,10 +2137,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2004,77 +2154,77 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B7" t="s">
         <v>267</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>268</v>
       </c>
-      <c r="C7" t="s">
-        <v>269</v>
-      </c>
       <c r="D7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>259</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>260</v>
-      </c>
       <c r="D9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>338</v>
+      </c>
+      <c r="B10" t="s">
         <v>339</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="29" t="s">
         <v>340</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>341</v>
-      </c>
       <c r="D10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2088,7 +2238,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2099,38 +2249,38 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>330</v>
+      </c>
+      <c r="B13" t="s">
         <v>331</v>
       </c>
-      <c r="B13" t="s">
-        <v>332</v>
-      </c>
       <c r="C13" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -2192,10 +2342,10 @@
         <v>0.71875</v>
       </c>
       <c r="D2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2209,10 +2359,10 @@
         <v>0.4375</v>
       </c>
       <c r="D4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2226,10 +2376,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2243,10 +2393,10 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2260,10 +2410,10 @@
         <v>0.4375</v>
       </c>
       <c r="D10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2277,10 +2427,10 @@
         <v>0.71875</v>
       </c>
       <c r="D11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2294,10 +2444,10 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="D13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2310,7 +2460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -2505,7 +2655,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E8" t="s">
         <v>65</v>
@@ -2807,7 +2957,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D24" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E24" t="s">
         <v>65</v>
@@ -2940,7 +3090,7 @@
         <v>159</v>
       </c>
       <c r="E30" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F30" t="s">
         <v>139</v>
@@ -2963,10 +3113,10 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D31" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E31" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G31" t="s">
         <v>140</v>
@@ -3116,7 +3266,7 @@
         <v>166</v>
       </c>
       <c r="E38" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F38" t="s">
         <v>139</v>
@@ -3268,8 +3418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3325,7 +3475,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E3" t="s">
         <v>77</v>
@@ -3342,10 +3492,10 @@
         <v>0.5625</v>
       </c>
       <c r="D4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3359,7 +3509,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E5" t="s">
         <v>213</v>
@@ -3411,10 +3561,10 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1">
@@ -3428,7 +3578,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>78</v>
@@ -3445,7 +3595,7 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>98</v>
@@ -3462,10 +3612,10 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>361</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1">
@@ -3479,7 +3629,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>218</v>
@@ -3496,7 +3646,7 @@
         <v>0.4375</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>218</v>
@@ -3513,7 +3663,7 @@
         <v>0.375</v>
       </c>
       <c r="D16" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>27</v>
@@ -3530,7 +3680,7 @@
         <v>0.4375</v>
       </c>
       <c r="D17" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>215</v>
@@ -3547,7 +3697,7 @@
         <v>0.5</v>
       </c>
       <c r="D18" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>216</v>
@@ -3564,7 +3714,7 @@
         <v>0.5625</v>
       </c>
       <c r="D19" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>218</v>
@@ -3581,7 +3731,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D20" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E20" s="32" t="s">
         <v>213</v>
@@ -3598,7 +3748,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D21" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>222</v>
@@ -3615,7 +3765,7 @@
         <v>0.84375</v>
       </c>
       <c r="D22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>76</v>
@@ -3666,7 +3816,7 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="D26" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>78</v>
@@ -3683,7 +3833,7 @@
         <v>0.57291666666666663</v>
       </c>
       <c r="D27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>218</v>
@@ -3700,10 +3850,10 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D28" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3717,7 +3867,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D30" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>219</v>
@@ -3734,7 +3884,7 @@
         <v>0.5</v>
       </c>
       <c r="D31" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>51</v>
@@ -3751,7 +3901,7 @@
         <v>0.57291666666666663</v>
       </c>
       <c r="D32" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>220</v>
@@ -3768,7 +3918,7 @@
         <v>0.4375</v>
       </c>
       <c r="D34" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>215</v>
@@ -3785,7 +3935,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="D35" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>221</v>
@@ -3802,10 +3952,10 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3819,7 +3969,7 @@
         <v>0.71875</v>
       </c>
       <c r="D38" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E38" s="32" t="s">
         <v>217</v>
@@ -3863,7 +4013,7 @@
         <v>44</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3877,13 +4027,13 @@
         <v>0.4375</v>
       </c>
       <c r="D2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3897,7 +4047,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -3914,7 +4064,7 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -3931,10 +4081,10 @@
         <v>0.8125</v>
       </c>
       <c r="D6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3948,10 +4098,10 @@
         <v>0.4375</v>
       </c>
       <c r="D8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E8" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3965,7 +4115,7 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -3982,10 +4132,10 @@
         <v>0.8125</v>
       </c>
       <c r="D11" t="s">
+        <v>333</v>
+      </c>
+      <c r="E11" t="s">
         <v>334</v>
-      </c>
-      <c r="E11" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3999,10 +4149,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4016,10 +4166,10 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="D14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4037,10 +4187,10 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="D16" t="s">
+        <v>333</v>
+      </c>
+      <c r="E16" t="s">
         <v>334</v>
-      </c>
-      <c r="E16" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -4054,10 +4204,10 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D18" t="s">
+        <v>336</v>
+      </c>
+      <c r="E18" t="s">
         <v>337</v>
-      </c>
-      <c r="E18" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4071,10 +4221,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -4129,13 +4279,13 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="D2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E2" t="s">
         <v>308</v>
       </c>
-      <c r="E2" t="s">
-        <v>309</v>
-      </c>
       <c r="G2" s="30" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
@@ -4151,13 +4301,13 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D3" t="s">
+        <v>309</v>
+      </c>
+      <c r="E3" t="s">
         <v>310</v>
       </c>
-      <c r="E3" t="s">
-        <v>311</v>
-      </c>
       <c r="G3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4171,10 +4321,10 @@
         <v>0.84375</v>
       </c>
       <c r="D4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4188,7 +4338,7 @@
         <v>0.40625</v>
       </c>
       <c r="D6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E6" t="s">
         <v>184</v>
@@ -4205,10 +4355,10 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="D7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4222,10 +4372,10 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="D8" t="s">
+        <v>314</v>
+      </c>
+      <c r="E8" t="s">
         <v>315</v>
-      </c>
-      <c r="E8" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4239,10 +4389,10 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="D10" t="s">
+        <v>316</v>
+      </c>
+      <c r="E10" t="s">
         <v>317</v>
-      </c>
-      <c r="E10" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4256,10 +4406,10 @@
         <v>0.625</v>
       </c>
       <c r="D11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -4273,10 +4423,10 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="D12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -4290,10 +4440,10 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -4307,10 +4457,10 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="D15" t="s">
+        <v>314</v>
+      </c>
+      <c r="E15" t="s">
         <v>315</v>
-      </c>
-      <c r="E15" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -4324,10 +4474,10 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="D17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -4341,10 +4491,10 @@
         <v>0.625</v>
       </c>
       <c r="D18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4358,10 +4508,10 @@
         <v>0.84375</v>
       </c>
       <c r="D19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -4375,10 +4525,10 @@
         <v>0.40625</v>
       </c>
       <c r="D21" t="s">
+        <v>322</v>
+      </c>
+      <c r="E21" t="s">
         <v>323</v>
-      </c>
-      <c r="E21" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -4392,10 +4542,10 @@
         <v>0.5</v>
       </c>
       <c r="D22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -4409,10 +4559,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -4426,10 +4576,10 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D25" t="s">
+        <v>325</v>
+      </c>
+      <c r="E25" t="s">
         <v>326</v>
-      </c>
-      <c r="E25" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -4443,10 +4593,10 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -4460,7 +4610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
@@ -4835,7 +4985,7 @@
         <v>0.71875</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>32</v>
@@ -4871,7 +5021,7 @@
         <v>0.8125</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>175</v>
@@ -4999,7 +5149,7 @@
         <v>227</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F32" s="29"/>
     </row>
@@ -5014,7 +5164,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D33" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E33" s="32" t="s">
         <v>37</v>
@@ -5359,7 +5509,7 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="D53" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>173</v>
@@ -5398,7 +5548,7 @@
         <v>232</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F55" s="29"/>
     </row>
@@ -5456,10 +5606,10 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D60" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F60" s="31"/>
     </row>
@@ -5474,7 +5624,7 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D61" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>37</v>
@@ -5492,7 +5642,7 @@
         <v>0.5625</v>
       </c>
       <c r="D62" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>197</v>
@@ -5510,7 +5660,7 @@
         <v>0.64930555555555558</v>
       </c>
       <c r="D63" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>198</v>
@@ -5528,7 +5678,7 @@
         <v>0.71875</v>
       </c>
       <c r="D64" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>199</v>
@@ -5546,7 +5696,7 @@
         <v>0.71875</v>
       </c>
       <c r="D65" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>198</v>
@@ -5564,7 +5714,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D66" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>17</v>
@@ -5598,7 +5748,7 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D69" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>201</v>
@@ -5616,7 +5766,7 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D70" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>32</v>
@@ -5634,7 +5784,7 @@
         <v>0.57291666666666663</v>
       </c>
       <c r="D71" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>39</v>
@@ -5670,7 +5820,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D73" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>189</v>
@@ -5691,7 +5841,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D75" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>179</v>
@@ -5708,7 +5858,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="D76" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>35</v>
@@ -5726,7 +5876,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D77" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>193</v>
@@ -5744,7 +5894,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="D78" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>194</v>
@@ -5762,7 +5912,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D79" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>37</v>
@@ -5780,7 +5930,7 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="D80" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>203</v>
@@ -5841,7 +5991,7 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="D2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E2" t="s">
         <v>172</v>
@@ -5860,10 +6010,10 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="D3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="15"/>
@@ -5882,10 +6032,10 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="D4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
@@ -5904,10 +6054,10 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="15"/>
@@ -5926,10 +6076,10 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="D6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E6" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="15"/>
@@ -5948,7 +6098,7 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E7" t="s">
         <v>172</v>
@@ -6849,10 +6999,10 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D43" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E43" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -6866,10 +7016,10 @@
         <v>0.84375</v>
       </c>
       <c r="D44" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E44" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6883,7 +7033,7 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="D45" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E45" t="s">
         <v>89</v>
@@ -6903,7 +7053,7 @@
         <v>117</v>
       </c>
       <c r="E47" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -7192,7 +7342,7 @@
         <v>132</v>
       </c>
       <c r="E66" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -7254,20 +7404,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="C58" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD79"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="91.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -7283,1295 +7433,619 @@
       <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="32" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="7">
-        <v>0.28125</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="C2" s="7">
-        <v>0.32291666666666669</v>
+        <v>0.40625</v>
       </c>
       <c r="D2" t="s">
-        <v>204</v>
+        <v>437</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="29"/>
-    </row>
-    <row r="3" spans="1:8">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="32" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="7">
-        <v>0.39583333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C3" s="7">
-        <v>0.45833333333333331</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="D3" t="s">
-        <v>205</v>
+        <v>421</v>
       </c>
       <c r="E3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="32" t="s">
         <v>80</v>
       </c>
       <c r="B4" s="7">
-        <v>0.41666666666666669</v>
+        <v>0.5</v>
       </c>
       <c r="C4" s="7">
-        <v>0.47916666666666669</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>422</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="32" t="s">
         <v>80</v>
       </c>
       <c r="B5" s="7">
-        <v>0.48958333333333331</v>
+        <v>0.5625</v>
       </c>
       <c r="C5" s="7">
-        <v>0.53125</v>
+        <v>0.625</v>
       </c>
       <c r="D5" t="s">
-        <v>206</v>
+        <v>423</v>
       </c>
       <c r="E5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="32" t="s">
         <v>80</v>
       </c>
       <c r="B6" s="7">
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C6" s="7">
-        <v>0.55208333333333337</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="D6" t="s">
-        <v>207</v>
+        <v>424</v>
       </c>
       <c r="E6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="32" t="s">
         <v>80</v>
       </c>
       <c r="B7" s="7">
-        <v>0.59375</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="C7" s="7">
-        <v>0.64583333333333337</v>
+        <v>0.78125</v>
       </c>
       <c r="D7" t="s">
-        <v>208</v>
+        <v>425</v>
       </c>
       <c r="E7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="32" t="s">
         <v>80</v>
       </c>
       <c r="B8" s="7">
-        <v>0.66666666666666663</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C8" s="7">
-        <v>0.71875</v>
+        <v>0.84375</v>
       </c>
       <c r="D8" t="s">
-        <v>209</v>
+        <v>441</v>
       </c>
       <c r="E8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="7">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="C9" s="7">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="D9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" s="7">
-        <v>0.75</v>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="34">
+        <v>0.35416666666666669</v>
       </c>
       <c r="C10" s="7">
-        <v>0.8125</v>
+        <v>0.40625</v>
       </c>
       <c r="D10" t="s">
-        <v>211</v>
+        <v>443</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="7">
-        <v>0.77083333333333337</v>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="35">
+        <v>0.41666666666666669</v>
       </c>
       <c r="C11" s="7">
-        <v>0.82291666666666663</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>445</v>
       </c>
       <c r="E11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="7">
-        <v>0.83333333333333337</v>
+        <v>446</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="35">
+        <v>0.5</v>
       </c>
       <c r="C12" s="7">
-        <v>0.88541666666666663</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D12" t="s">
-        <v>212</v>
+        <v>447</v>
       </c>
       <c r="E12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1"/>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A14" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2">
-        <v>0.28125</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.32291666666666669</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="29"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B13" s="35">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D13" t="s">
+        <v>448</v>
+      </c>
+      <c r="E13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="35">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D14" t="s">
+        <v>425</v>
+      </c>
+      <c r="E14" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5">
-        <v>0.34375</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0.38541666666666669</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="29"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B15" s="35">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="D15" t="s">
+        <v>425</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="35">
+        <v>0.8125</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D16" t="s">
+        <v>451</v>
+      </c>
+      <c r="E16" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="7">
         <v>0.375</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C18" s="7">
         <v>0.42708333333333331</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="29"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="5">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="29"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="5">
+      <c r="D18" t="s">
+        <v>453</v>
+      </c>
+      <c r="E18" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="7">
         <v>0.4375</v>
       </c>
-      <c r="C18" s="5">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="29"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="5">
+      <c r="C19" s="7">
         <v>0.5</v>
       </c>
-      <c r="C19" s="5">
+      <c r="D19" t="s">
+        <v>455</v>
+      </c>
+      <c r="E19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D20" t="s">
+        <v>457</v>
+      </c>
+      <c r="E20" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D21" t="s">
+        <v>422</v>
+      </c>
+      <c r="E21" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D22" t="s">
+        <v>441</v>
+      </c>
+      <c r="E22" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D23" t="s">
+        <v>422</v>
+      </c>
+      <c r="E23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0.78125</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.84375</v>
+      </c>
+      <c r="D24" t="s">
+        <v>426</v>
+      </c>
+      <c r="E24" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0.40625</v>
+      </c>
+      <c r="D26" t="s">
+        <v>422</v>
+      </c>
+      <c r="E26" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="7">
+        <v>0.4375</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D27" t="s">
+        <v>462</v>
+      </c>
+      <c r="E27" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D28" t="s">
+        <v>428</v>
+      </c>
+      <c r="E28" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="7">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0.625</v>
+      </c>
+      <c r="D29" t="s">
+        <v>463</v>
+      </c>
+      <c r="E29" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D30" t="s">
+        <v>429</v>
+      </c>
+      <c r="E30" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="D31" t="s">
+        <v>466</v>
+      </c>
+      <c r="E31" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C32" s="7">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D32" t="s">
+        <v>467</v>
+      </c>
+      <c r="E32" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D34" t="s">
+        <v>468</v>
+      </c>
+      <c r="E34" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D35" t="s">
+        <v>430</v>
+      </c>
+      <c r="E35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D36" t="s">
+        <v>431</v>
+      </c>
+      <c r="E36" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C37" s="7">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="29"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="5">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="C20" s="5">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="29"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="5">
+      <c r="D37" t="s">
+        <v>433</v>
+      </c>
+      <c r="E37" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="7">
         <v>0.5625</v>
       </c>
-      <c r="C21" s="5">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="29"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="5">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C22" s="5">
-        <v>0.71875</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="29"/>
-    </row>
-    <row r="23" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="5">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="31"/>
-    </row>
-    <row r="24" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="5">
+      <c r="C38" s="7">
+        <v>0.625</v>
+      </c>
+      <c r="D38" t="s">
+        <v>434</v>
+      </c>
+      <c r="E38" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="7">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="D40" t="s">
+        <v>435</v>
+      </c>
+      <c r="E40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="7">
         <v>0.75</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C41" s="7">
         <v>0.8125</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="F24" s="31"/>
-    </row>
-    <row r="25" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0.80902777777777779</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="31"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="5">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C26" s="5">
-        <v>0.89583333333333337</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="29"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="7">
-        <v>0.28125</v>
-      </c>
-      <c r="C28" s="7">
-        <v>0.32291666666666669</v>
-      </c>
-      <c r="D28" t="s">
-        <v>204</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="7">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C29" s="7">
-        <v>0.38541666666666669</v>
-      </c>
-      <c r="D29" t="s">
-        <v>224</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="F29" s="29"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="7">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="C30" s="7">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D30" t="s">
-        <v>225</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="F30" s="29"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="7">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C31" s="7">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D31" t="s">
-        <v>226</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="F31" s="29"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="7">
-        <v>0.46875</v>
-      </c>
-      <c r="C32" s="7">
-        <v>0.48958333333333331</v>
-      </c>
-      <c r="D32" t="s">
-        <v>227</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>182</v>
-      </c>
-      <c r="F32" s="29"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75">
-      <c r="A33" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="C33" s="7">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D33" t="s">
-        <v>368</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" s="31"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75">
-      <c r="A34" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="7">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="C34" s="7">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="D34" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="32" t="s">
-        <v>183</v>
-      </c>
-      <c r="F34" s="31"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75">
-      <c r="A35" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="7">
-        <v>0.59375</v>
-      </c>
-      <c r="C35" s="7">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="D35" t="s">
-        <v>228</v>
-      </c>
-      <c r="E35" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="F35" s="31"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75">
-      <c r="A36" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="7">
-        <v>0.59375</v>
-      </c>
-      <c r="C36" s="7">
-        <v>0.63541666666666663</v>
-      </c>
-      <c r="D36" t="s">
-        <v>229</v>
-      </c>
-      <c r="E36" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="F36" s="31"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37" s="7">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C37" s="7">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="D37" t="s">
-        <v>230</v>
-      </c>
-      <c r="E37" s="32" t="s">
-        <v>187</v>
-      </c>
-      <c r="F37" s="29"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" s="7">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C38" s="7">
-        <v>0.71875</v>
-      </c>
-      <c r="D38" t="s">
-        <v>231</v>
-      </c>
-      <c r="E38" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="F38" s="29"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75">
-      <c r="A39" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="7">
-        <v>0.71875</v>
-      </c>
-      <c r="C39" s="7">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="D39" t="s">
-        <v>232</v>
-      </c>
-      <c r="E39" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="F39" s="31"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="7">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="C40" s="7">
+      <c r="D41" t="s">
+        <v>422</v>
+      </c>
+      <c r="E41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="7">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D40" t="s">
-        <v>233</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F40" s="29"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="7">
-        <v>0.82291666666666663</v>
-      </c>
-      <c r="C41" s="7">
-        <v>0.875</v>
-      </c>
-      <c r="D41" t="s">
-        <v>232</v>
-      </c>
-      <c r="E41" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="F41" s="29"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="7">
-        <v>0.83333333333333337</v>
-      </c>
       <c r="C42" s="7">
-        <v>0.89583333333333337</v>
+        <v>0.86458333333333337</v>
       </c>
       <c r="D42" t="s">
-        <v>234</v>
-      </c>
-      <c r="E42" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="F42" s="29"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="C44" s="7">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D44" t="s">
-        <v>235</v>
-      </c>
-      <c r="E44" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F44" s="29"/>
-    </row>
-    <row r="45" spans="1:6" ht="15.75">
-      <c r="A45" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" s="7">
-        <v>0.30208333333333331</v>
-      </c>
-      <c r="C45" s="7">
-        <v>0.34375</v>
-      </c>
-      <c r="D45" t="s">
-        <v>236</v>
-      </c>
-      <c r="E45" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="F45" s="31"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="7">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="C46" s="7">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D46" t="s">
-        <v>238</v>
-      </c>
-      <c r="E46" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="F46" s="29"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47" s="7">
-        <v>0.46875</v>
-      </c>
-      <c r="C47" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="D47" t="s">
-        <v>415</v>
-      </c>
-      <c r="E47" s="32" t="s">
-        <v>182</v>
-      </c>
-      <c r="F47" s="29"/>
-    </row>
-    <row r="48" spans="1:6" ht="15.75">
-      <c r="A48" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="C48" s="7">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D48" t="s">
-        <v>26</v>
-      </c>
-      <c r="E48" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="F48" s="31"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49" s="7">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="C49" s="7">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="D49" t="s">
-        <v>239</v>
-      </c>
-      <c r="E49" s="32" t="s">
-        <v>192</v>
-      </c>
-      <c r="F49" s="29"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B50" s="7">
-        <v>0.59375</v>
-      </c>
-      <c r="C50" s="7">
-        <v>0.64930555555555558</v>
-      </c>
-      <c r="D50" t="s">
-        <v>240</v>
-      </c>
-      <c r="E50" s="32" t="s">
-        <v>193</v>
-      </c>
-      <c r="F50" s="29"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B51" s="7">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C51" s="7">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="D51" t="s">
-        <v>26</v>
-      </c>
-      <c r="E51" s="32" t="s">
-        <v>194</v>
-      </c>
-      <c r="F51" s="29"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B52" s="7">
-        <v>0.6875</v>
-      </c>
-      <c r="C52" s="7">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="D52" t="s">
-        <v>241</v>
-      </c>
-      <c r="E52" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="F52" s="29"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="7">
-        <v>0.71875</v>
-      </c>
-      <c r="C53" s="7">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="D53" t="s">
-        <v>368</v>
-      </c>
-      <c r="E53" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="F53" s="29"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" s="7">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="C54" s="7">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D54" t="s">
-        <v>26</v>
-      </c>
-      <c r="E54" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F54" s="29"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" s="7">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C55" s="7">
-        <v>0.89583333333333337</v>
-      </c>
-      <c r="D55" t="s">
-        <v>232</v>
-      </c>
-      <c r="E55" s="32" t="s">
-        <v>193</v>
-      </c>
-      <c r="F55" s="29"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="7">
-        <v>0.84375</v>
-      </c>
-      <c r="C56" s="7">
-        <v>0.89583333333333337</v>
-      </c>
-      <c r="D56" t="s">
-        <v>242</v>
-      </c>
-      <c r="E56" s="32" t="s">
-        <v>196</v>
-      </c>
-      <c r="F56" s="29"/>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B58" s="7">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="C58" s="7">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D58" t="s">
-        <v>243</v>
-      </c>
-      <c r="E58" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F58" s="29"/>
-    </row>
-    <row r="59" spans="1:6" ht="15.75">
-      <c r="A59" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B59" s="7">
-        <v>0.46875</v>
-      </c>
-      <c r="C59" s="7">
-        <v>0.48958333333333331</v>
-      </c>
-      <c r="D59" t="s">
-        <v>244</v>
-      </c>
-      <c r="E59" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="F59" s="31"/>
-    </row>
-    <row r="60" spans="1:6" ht="15.75">
-      <c r="A60" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B60" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="C60" s="7">
-        <v>0.55208333333333337</v>
-      </c>
-      <c r="D60" t="s">
-        <v>245</v>
-      </c>
-      <c r="E60" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F60" s="31"/>
-    </row>
-    <row r="61" spans="1:6" ht="15.75">
-      <c r="A61" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B61" s="7">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="C61" s="7">
-        <v>0.5625</v>
-      </c>
-      <c r="D61" t="s">
-        <v>369</v>
-      </c>
-      <c r="E61" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="F61" s="31"/>
-    </row>
-    <row r="62" spans="1:6" ht="15.75">
-      <c r="A62" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B62" s="7">
-        <v>0.59375</v>
-      </c>
-      <c r="C62" s="7">
-        <v>0.64930555555555558</v>
-      </c>
-      <c r="D62" t="s">
-        <v>370</v>
-      </c>
-      <c r="E62" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="F62" s="31"/>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B63" s="7">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C63" s="7">
-        <v>0.71875</v>
-      </c>
-      <c r="D63" t="s">
-        <v>246</v>
-      </c>
-      <c r="E63" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="F63" s="29"/>
-    </row>
-    <row r="64" spans="1:6" ht="15.75">
-      <c r="A64" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B64" s="7">
-        <v>0.67708333333333337</v>
-      </c>
-      <c r="C64" s="7">
-        <v>0.71875</v>
-      </c>
-      <c r="D64" t="s">
-        <v>247</v>
-      </c>
-      <c r="E64" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="F64" s="31"/>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B65" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="C65" s="7">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="D65" t="s">
-        <v>245</v>
-      </c>
-      <c r="E65" s="32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B67" s="7">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="C67" s="7">
-        <v>0.40625</v>
-      </c>
-      <c r="D67" t="s">
-        <v>26</v>
-      </c>
-      <c r="E67" s="32" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B68" s="7">
-        <v>0.42708333333333331</v>
-      </c>
-      <c r="C68" s="7">
-        <v>0.48958333333333331</v>
-      </c>
-      <c r="D68" t="s">
-        <v>248</v>
-      </c>
-      <c r="E68" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="F68" s="29"/>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B69" s="7">
-        <v>0.4375</v>
-      </c>
-      <c r="C69" s="7">
-        <v>0.48958333333333331</v>
-      </c>
-      <c r="D69" t="s">
-        <v>26</v>
-      </c>
-      <c r="E69" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="F69" s="29"/>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B70" s="7">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="C70" s="7">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="D70" t="s">
-        <v>249</v>
-      </c>
-      <c r="E70" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="F70" s="29"/>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B71" s="7">
-        <v>0.59375</v>
-      </c>
-      <c r="C71" s="7">
-        <v>0.63541666666666663</v>
-      </c>
-      <c r="D71" t="s">
-        <v>243</v>
-      </c>
-      <c r="E71" s="32" t="s">
-        <v>202</v>
-      </c>
-      <c r="F71" s="29"/>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B72" s="7">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="C72" s="7">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="D72" t="s">
-        <v>249</v>
-      </c>
-      <c r="E72" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="F72" s="29"/>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="F73" s="29"/>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B74" s="7">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="C74" s="7">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D74" t="s">
-        <v>250</v>
-      </c>
-      <c r="E74" s="32" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B75" s="7">
-        <v>0.46875</v>
-      </c>
-      <c r="C75" s="7">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="D75" t="s">
-        <v>251</v>
-      </c>
-      <c r="E75" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F75" s="29"/>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B76" s="7">
-        <v>0.53125</v>
-      </c>
-      <c r="C76" s="7">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="D76" t="s">
-        <v>252</v>
-      </c>
-      <c r="E76" s="32" t="s">
-        <v>193</v>
-      </c>
-      <c r="F76" s="29"/>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B77" s="7">
-        <v>0.59375</v>
-      </c>
-      <c r="C77" s="7">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="D77" t="s">
-        <v>253</v>
-      </c>
-      <c r="E77" s="32" t="s">
-        <v>194</v>
-      </c>
-      <c r="F77" s="29"/>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B78" s="7">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C78" s="7">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="D78" t="s">
-        <v>254</v>
-      </c>
-      <c r="E78" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F78" s="29"/>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="C79" s="7">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="D79" t="s">
-        <v>255</v>
-      </c>
-      <c r="E79" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="F79" s="29"/>
+        <v>436</v>
+      </c>
+      <c r="E42" t="s">
+        <v>411</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -8622,7 +8096,7 @@
         <v>0.84375</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E2" t="s">
         <v>147</v>
@@ -8639,7 +8113,7 @@
         <v>0.4375</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E3" t="s">
         <v>147</v>
@@ -8656,7 +8130,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E4" t="s">
         <v>147</v>
@@ -8713,10 +8187,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75">
@@ -8730,10 +8204,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75">
@@ -8752,10 +8226,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75">
@@ -8769,10 +8243,10 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="D6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75">
@@ -8791,10 +8265,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75">
@@ -8808,10 +8282,10 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="D9" t="s">
+        <v>302</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>303</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75">
@@ -8830,10 +8304,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D11" t="s">
+        <v>302</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>303</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75">
@@ -8850,7 +8324,7 @@
         <v>108</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75">
@@ -8869,10 +8343,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75">
@@ -8947,10 +8421,10 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="D2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E2" t="s">
         <v>284</v>
-      </c>
-      <c r="E2" t="s">
-        <v>285</v>
       </c>
       <c r="H2"/>
       <c r="I2"/>
@@ -8966,10 +8440,10 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="33"/>
@@ -8987,10 +8461,10 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" t="s">
         <v>287</v>
-      </c>
-      <c r="E4" t="s">
-        <v>288</v>
       </c>
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
@@ -9008,10 +8482,10 @@
         <v>0.78125</v>
       </c>
       <c r="D5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -9037,10 +8511,10 @@
         <v>0.3125</v>
       </c>
       <c r="D7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E7" t="s">
         <v>284</v>
-      </c>
-      <c r="E7" t="s">
-        <v>285</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="28"/>
@@ -9058,10 +8532,10 @@
         <v>0.46875</v>
       </c>
       <c r="D8" t="s">
+        <v>289</v>
+      </c>
+      <c r="E8" t="s">
         <v>290</v>
-      </c>
-      <c r="E8" t="s">
-        <v>291</v>
       </c>
       <c r="G8" s="26"/>
       <c r="H8" s="28"/>
@@ -9079,10 +8553,10 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
@@ -9100,10 +8574,10 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="D10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G10" s="26"/>
       <c r="H10" s="28"/>
@@ -9129,10 +8603,10 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="D12" t="s">
+        <v>283</v>
+      </c>
+      <c r="E12" t="s">
         <v>284</v>
-      </c>
-      <c r="E12" t="s">
-        <v>285</v>
       </c>
       <c r="G12" s="26"/>
       <c r="H12" s="28"/>
@@ -9150,10 +8624,10 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="28"/>
@@ -9171,10 +8645,10 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
@@ -9192,10 +8666,10 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G15" s="26"/>
       <c r="H15" s="28"/>
@@ -9221,10 +8695,10 @@
         <v>0.3125</v>
       </c>
       <c r="D17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="28"/>
@@ -9242,10 +8716,10 @@
         <v>0.46875</v>
       </c>
       <c r="D18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G18" s="26"/>
       <c r="H18" s="28"/>
@@ -9263,10 +8737,10 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G19" s="33"/>
       <c r="H19" s="33"/>
@@ -9284,10 +8758,10 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="D20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G20" s="26"/>
       <c r="H20" s="28"/>
@@ -9313,10 +8787,10 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="D22" t="s">
+        <v>283</v>
+      </c>
+      <c r="E22" t="s">
         <v>284</v>
-      </c>
-      <c r="E22" t="s">
-        <v>285</v>
       </c>
       <c r="G22" s="26"/>
       <c r="H22" s="28"/>
@@ -9334,7 +8808,7 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E23" t="s">
         <v>172</v>
@@ -9355,10 +8829,10 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G24" s="26"/>
       <c r="H24" s="28"/>
@@ -9376,10 +8850,10 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D25" t="s">
+        <v>283</v>
+      </c>
+      <c r="E25" t="s">
         <v>284</v>
-      </c>
-      <c r="E25" t="s">
-        <v>285</v>
       </c>
       <c r="G25" s="26"/>
       <c r="H25" s="28"/>
@@ -9405,10 +8879,10 @@
         <v>0.46875</v>
       </c>
       <c r="D27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G27" s="26"/>
       <c r="H27" s="28"/>
@@ -9426,10 +8900,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E28" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G28" s="26"/>
       <c r="H28" s="28"/>
@@ -9455,10 +8929,10 @@
         <v>0.46875</v>
       </c>
       <c r="D30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G30" s="26"/>
       <c r="H30" s="28"/>
@@ -9476,10 +8950,10 @@
         <v>0.46875</v>
       </c>
       <c r="D31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G31" s="33"/>
       <c r="H31" s="33"/>
@@ -9571,7 +9045,7 @@
         <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -9585,10 +9059,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -9602,10 +9076,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -9619,10 +9093,10 @@
         <v>0.5625</v>
       </c>
       <c r="D4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -9636,10 +9110,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E5" t="s">
         <v>277</v>
-      </c>
-      <c r="E5" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -9653,10 +9127,10 @@
         <v>0.75</v>
       </c>
       <c r="D6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -9670,10 +9144,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -9690,10 +9164,10 @@
         <v>0.32291666666666669</v>
       </c>
       <c r="D9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -9707,10 +9181,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -9724,10 +9198,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D11" t="s">
+        <v>273</v>
+      </c>
+      <c r="E11" t="s">
         <v>274</v>
-      </c>
-      <c r="E11" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -9741,10 +9215,10 @@
         <v>0.75</v>
       </c>
       <c r="D12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -9758,10 +9232,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -9778,10 +9252,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -9795,10 +9269,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -9812,10 +9286,10 @@
         <v>0.5625</v>
       </c>
       <c r="D17" t="s">
+        <v>273</v>
+      </c>
+      <c r="E17" t="s">
         <v>274</v>
-      </c>
-      <c r="E17" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -9829,10 +9303,10 @@
         <v>0.75</v>
       </c>
       <c r="D18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -9846,10 +9320,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -9866,10 +9340,10 @@
         <v>0.32291666666666669</v>
       </c>
       <c r="D21" t="s">
+        <v>273</v>
+      </c>
+      <c r="E21" t="s">
         <v>274</v>
-      </c>
-      <c r="E21" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -9883,10 +9357,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -9900,10 +9374,10 @@
         <v>0.5625</v>
       </c>
       <c r="D23" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -9917,10 +9391,10 @@
         <v>0.75</v>
       </c>
       <c r="D24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -9934,10 +9408,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -9954,10 +9428,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -9971,10 +9445,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -9988,10 +9462,10 @@
         <v>0.5625</v>
       </c>
       <c r="D29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E29" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -10005,10 +9479,10 @@
         <v>0.75</v>
       </c>
       <c r="D30" t="s">
+        <v>273</v>
+      </c>
+      <c r="E30" t="s">
         <v>274</v>
-      </c>
-      <c r="E30" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -10022,10 +9496,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -10042,10 +9516,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D33" t="s">
+        <v>273</v>
+      </c>
+      <c r="E33" t="s">
         <v>274</v>
-      </c>
-      <c r="E33" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -10059,10 +9533,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -10076,10 +9550,10 @@
         <v>0.5625</v>
       </c>
       <c r="D35" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E35" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -10093,10 +9567,10 @@
         <v>0.75</v>
       </c>
       <c r="D36" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -10113,10 +9587,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -10130,10 +9604,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -10147,10 +9621,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D40" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E40" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -10164,10 +9638,10 @@
         <v>0.75</v>
       </c>
       <c r="D41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Urban Ashram Studio
</commit_message>
<xml_diff>
--- a/AvlZen/App_Data/AvlZen.xlsx
+++ b/AvlZen/App_Data/AvlZen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="-15" windowWidth="15645" windowHeight="12060" tabRatio="907" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="7440" yWindow="-15" windowWidth="15645" windowHeight="12060" tabRatio="907" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Places" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="HotYogAvl" sheetId="7" r:id="rId9"/>
     <sheet name="NrshLifeCtr" sheetId="15" r:id="rId10"/>
     <sheet name="OneCtrYog" sheetId="5" r:id="rId11"/>
-    <sheet name="WstAvlYog" sheetId="6" r:id="rId12"/>
-    <sheet name="YmcaReut" sheetId="14" r:id="rId13"/>
-    <sheet name="YmcaWdfn" sheetId="13" r:id="rId14"/>
+    <sheet name="UrbAshram" sheetId="16" r:id="rId12"/>
+    <sheet name="WstAvlYog" sheetId="6" r:id="rId13"/>
+    <sheet name="YmcaReut" sheetId="14" r:id="rId14"/>
+    <sheet name="YmcaWdfn" sheetId="13" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_cid31" localSheetId="2">AvlHapBod!$J$3</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="500">
   <si>
     <t>Code</t>
   </si>
@@ -1469,6 +1470,90 @@
   </si>
   <si>
     <t>Jackie Dobrinska</t>
+  </si>
+  <si>
+    <t>UrbAshram</t>
+  </si>
+  <si>
+    <t>Urban Ashram Studio</t>
+  </si>
+  <si>
+    <t>https://clients.mindbodyonline.com/ASP/home.asp?studioid=149266</t>
+  </si>
+  <si>
+    <t>62 Wall St Asheville, North Carolina 28801</t>
+  </si>
+  <si>
+    <t>Rise and Shine Vinyasa Flow - $10 Drop in</t>
+  </si>
+  <si>
+    <t>Lyle Mitchell</t>
+  </si>
+  <si>
+    <t>All Levels Vinyasa Flow</t>
+  </si>
+  <si>
+    <t>Lillian Jacobs</t>
+  </si>
+  <si>
+    <t>Power Hour - $10 Drop in</t>
+  </si>
+  <si>
+    <t>Level 1 Vinyasa Flow - $5 Drop in</t>
+  </si>
+  <si>
+    <t>Julian Albertson</t>
+  </si>
+  <si>
+    <t>Playful Flow</t>
+  </si>
+  <si>
+    <t>Rich Risbridger</t>
+  </si>
+  <si>
+    <t>Vin Yin Blend</t>
+  </si>
+  <si>
+    <t>Lea Mclellan</t>
+  </si>
+  <si>
+    <t>Heated Flow</t>
+  </si>
+  <si>
+    <t>Lia Curtis-Fine</t>
+  </si>
+  <si>
+    <t>All Levels Yoga</t>
+  </si>
+  <si>
+    <t>Eva Rose</t>
+  </si>
+  <si>
+    <t>Kick Your Asana</t>
+  </si>
+  <si>
+    <t>AcroYoga</t>
+  </si>
+  <si>
+    <t>The Roots</t>
+  </si>
+  <si>
+    <t>Emma Salmon</t>
+  </si>
+  <si>
+    <t>AcroYoga: Thai &amp; Fly</t>
+  </si>
+  <si>
+    <t>Level 1-2 Vinyasa Flow - $5 Drop in</t>
+  </si>
+  <si>
+    <t>AcroYoga Conditioning *Cancelled 4/27</t>
+  </si>
+  <si>
+    <t>Yin</t>
+  </si>
+  <si>
+    <t>Cara Mckinney</t>
   </si>
 </sst>
 </file>
@@ -1762,14 +1847,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2073,10 +2158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2243,43 +2328,57 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>472</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>473</v>
       </c>
       <c r="C12" t="s">
-        <v>257</v>
+        <v>474</v>
       </c>
       <c r="D12" t="s">
-        <v>349</v>
+        <v>475</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>330</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>331</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>372</v>
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>257</v>
       </c>
       <c r="D13" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B14" t="s">
-        <v>269</v>
+        <v>331</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>372</v>
       </c>
       <c r="D14" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>328</v>
+      </c>
+      <c r="B15" t="s">
+        <v>269</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="D15" t="s">
         <v>356</v>
       </c>
     </row>
@@ -2304,7 +2403,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3416,10 +3515,667 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.28125</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D2" t="s">
+        <v>476</v>
+      </c>
+      <c r="E2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D3" t="s">
+        <v>478</v>
+      </c>
+      <c r="E3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.53125</v>
+      </c>
+      <c r="D4" t="s">
+        <v>480</v>
+      </c>
+      <c r="E4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="D5" t="s">
+        <v>481</v>
+      </c>
+      <c r="E5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.78125</v>
+      </c>
+      <c r="D6" t="s">
+        <v>483</v>
+      </c>
+      <c r="E6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.84375</v>
+      </c>
+      <c r="D7" t="s">
+        <v>485</v>
+      </c>
+      <c r="E7" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D9" t="s">
+        <v>478</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.4375</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D10" t="s">
+        <v>487</v>
+      </c>
+      <c r="E10" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="D11" t="s">
+        <v>489</v>
+      </c>
+      <c r="E11" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.78125</v>
+      </c>
+      <c r="D12" t="s">
+        <v>491</v>
+      </c>
+      <c r="E12" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D13" t="s">
+        <v>492</v>
+      </c>
+      <c r="E13" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0.28125</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D15" t="s">
+        <v>476</v>
+      </c>
+      <c r="E15" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D16" t="s">
+        <v>478</v>
+      </c>
+      <c r="E16" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D17" t="s">
+        <v>480</v>
+      </c>
+      <c r="E17" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="D18" t="s">
+        <v>481</v>
+      </c>
+      <c r="E18" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.78125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>483</v>
+      </c>
+      <c r="E19" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.84375</v>
+      </c>
+      <c r="D20" t="s">
+        <v>485</v>
+      </c>
+      <c r="E20" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D22" t="s">
+        <v>478</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="7">
+        <v>0.4375</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D23" t="s">
+        <v>487</v>
+      </c>
+      <c r="E23" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="D24" t="s">
+        <v>489</v>
+      </c>
+      <c r="E24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="7">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.78125</v>
+      </c>
+      <c r="D25" t="s">
+        <v>491</v>
+      </c>
+      <c r="E25" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0.84375</v>
+      </c>
+      <c r="D26" t="s">
+        <v>493</v>
+      </c>
+      <c r="E26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0.28125</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D28" t="s">
+        <v>476</v>
+      </c>
+      <c r="E28" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D29" t="s">
+        <v>478</v>
+      </c>
+      <c r="E29" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D30" t="s">
+        <v>480</v>
+      </c>
+      <c r="E30" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="D31" t="s">
+        <v>481</v>
+      </c>
+      <c r="E31" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C32" s="7">
+        <v>0.78125</v>
+      </c>
+      <c r="D32" t="s">
+        <v>483</v>
+      </c>
+      <c r="E32" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="7">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0.84375</v>
+      </c>
+      <c r="D33" t="s">
+        <v>495</v>
+      </c>
+      <c r="E33" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D35" t="s">
+        <v>496</v>
+      </c>
+      <c r="E35" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D36" t="s">
+        <v>478</v>
+      </c>
+      <c r="E36" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D37" t="s">
+        <v>478</v>
+      </c>
+      <c r="E37" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="7">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D39" t="s">
+        <v>478</v>
+      </c>
+      <c r="E39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D40" t="s">
+        <v>478</v>
+      </c>
+      <c r="E40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="7">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C41" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D41" t="s">
+        <v>497</v>
+      </c>
+      <c r="E41" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="D42" t="s">
+        <v>498</v>
+      </c>
+      <c r="E42" t="s">
+        <v>499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3981,12 +4737,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4237,12 +4993,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4611,7 +5367,7 @@
   <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5952,7 +6708,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6313,7 +7069,7 @@
   <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7407,7 +8163,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7558,7 +8314,7 @@
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="34">
+      <c r="B10" s="33">
         <v>0.35416666666666669</v>
       </c>
       <c r="C10" s="7">
@@ -7575,7 +8331,7 @@
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="34">
         <v>0.41666666666666669</v>
       </c>
       <c r="C11" s="7">
@@ -7592,7 +8348,7 @@
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="34">
         <v>0.5</v>
       </c>
       <c r="C12" s="7">
@@ -7609,7 +8365,7 @@
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="35">
+      <c r="B13" s="34">
         <v>0.58333333333333337</v>
       </c>
       <c r="C13" s="7">
@@ -7626,7 +8382,7 @@
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14" s="34">
         <v>0.67708333333333337</v>
       </c>
       <c r="C14" s="7">
@@ -7643,7 +8399,7 @@
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="34">
         <v>0.73958333333333337</v>
       </c>
       <c r="C15" s="7">
@@ -7660,7 +8416,7 @@
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16" s="34">
         <v>0.8125</v>
       </c>
       <c r="C16" s="7">
@@ -8058,7 +8814,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8148,7 +8904,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:IV1"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8376,7 +9132,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8445,8 +9201,8 @@
       <c r="E3" t="s">
         <v>293</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
     </row>
@@ -8495,8 +9251,8 @@
     <row r="6" spans="1:10">
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
     </row>
@@ -8558,8 +9314,8 @@
       <c r="E9" t="s">
         <v>291</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
       <c r="I9" s="27"/>
       <c r="J9" s="27"/>
     </row>
@@ -8650,8 +9406,8 @@
       <c r="E14" t="s">
         <v>288</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
     </row>
@@ -8742,8 +9498,8 @@
       <c r="E19" t="s">
         <v>294</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
     </row>
@@ -8863,8 +9619,8 @@
     <row r="26" spans="1:10">
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
       <c r="I26" s="27"/>
       <c r="J26" s="27"/>
     </row>
@@ -8955,8 +9711,8 @@
       <c r="E31" t="s">
         <v>290</v>
       </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
       <c r="I31" s="27"/>
       <c r="J31" s="27"/>
     </row>
@@ -9017,7 +9773,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Logo and Link fixes
</commit_message>
<xml_diff>
--- a/AvlZen/App_Data/AvlZen.xlsx
+++ b/AvlZen/App_Data/AvlZen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="-15" windowWidth="15645" windowHeight="12060" tabRatio="907" firstSheet="8" activeTab="14"/>
+    <workbookView xWindow="7440" yWindow="-15" windowWidth="15645" windowHeight="12060" tabRatio="907"/>
   </bookViews>
   <sheets>
     <sheet name="Places" sheetId="1" r:id="rId1"/>
@@ -800,9 +800,6 @@
     <t>http://ashevillecommunityyoga.com/class-schedules/</t>
   </si>
   <si>
-    <t>http://westashevilleyoga.com/class-schedule/</t>
-  </si>
-  <si>
     <t>Hot Yoga Asheville</t>
   </si>
   <si>
@@ -1391,9 +1388,6 @@
     <t>Urban Ashram Studio</t>
   </si>
   <si>
-    <t>https://clients.mindbodyonline.com/ASP/home.asp?studioid=149266</t>
-  </si>
-  <si>
     <t>62 Wall St Asheville, North Carolina 28801</t>
   </si>
   <si>
@@ -1560,6 +1554,12 @@
   </si>
   <si>
     <t>Jane Anne</t>
+  </si>
+  <si>
+    <t>http://urbanashramstudio.com/</t>
+  </si>
+  <si>
+    <t>http://westashevilleyoga.com/schedule/</t>
   </si>
 </sst>
 </file>
@@ -2166,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2189,7 +2189,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2203,21 +2203,21 @@
         <v>247</v>
       </c>
       <c r="D2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" t="s">
         <v>254</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>255</v>
       </c>
-      <c r="C3" t="s">
-        <v>256</v>
-      </c>
       <c r="D3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2228,10 +2228,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2245,77 +2245,77 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>256</v>
+      </c>
+      <c r="B7" t="s">
         <v>257</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>258</v>
       </c>
-      <c r="C7" t="s">
-        <v>259</v>
-      </c>
       <c r="D7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>250</v>
-      </c>
       <c r="D9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>326</v>
+      </c>
+      <c r="B10" t="s">
         <v>327</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>329</v>
-      </c>
       <c r="D10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2329,21 +2329,21 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>442</v>
+      </c>
+      <c r="B12" t="s">
         <v>443</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>500</v>
+      </c>
+      <c r="D12" t="s">
         <v>444</v>
-      </c>
-      <c r="C12" t="s">
-        <v>445</v>
-      </c>
-      <c r="D12" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2353,39 +2353,39 @@
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
-        <v>248</v>
+      <c r="C13" s="29" t="s">
+        <v>501</v>
       </c>
       <c r="D13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>318</v>
+      </c>
+      <c r="B14" t="s">
         <v>319</v>
       </c>
-      <c r="B14" t="s">
-        <v>320</v>
-      </c>
       <c r="C14" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2398,9 +2398,10 @@
     <hyperlink ref="C4" r:id="rId2"/>
     <hyperlink ref="C8" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
+    <hyperlink ref="C13" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2447,10 +2448,10 @@
         <v>0.71875</v>
       </c>
       <c r="D2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2464,10 +2465,10 @@
         <v>0.4375</v>
       </c>
       <c r="D4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2481,10 +2482,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D6" t="s">
+        <v>361</v>
+      </c>
+      <c r="E6" t="s">
         <v>362</v>
-      </c>
-      <c r="E6" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2498,10 +2499,10 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="D7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2515,10 +2516,10 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D9" t="s">
+        <v>363</v>
+      </c>
+      <c r="E9" t="s">
         <v>364</v>
-      </c>
-      <c r="E9" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2532,10 +2533,10 @@
         <v>0.4375</v>
       </c>
       <c r="D11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -2743,7 +2744,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E8" t="s">
         <v>63</v>
@@ -2796,7 +2797,7 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>63</v>
@@ -2881,7 +2882,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>144</v>
@@ -3045,7 +3046,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D24" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E24" t="s">
         <v>63</v>
@@ -3152,7 +3153,7 @@
         <v>152</v>
       </c>
       <c r="E29" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F29" t="s">
         <v>133</v>
@@ -3175,10 +3176,10 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D30" t="s">
+        <v>367</v>
+      </c>
+      <c r="E30" t="s">
         <v>368</v>
-      </c>
-      <c r="E30" t="s">
-        <v>369</v>
       </c>
       <c r="G30" t="s">
         <v>134</v>
@@ -3328,7 +3329,7 @@
         <v>159</v>
       </c>
       <c r="E37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F37" t="s">
         <v>133</v>
@@ -3519,10 +3520,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3536,10 +3537,10 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3553,10 +3554,10 @@
         <v>0.53125</v>
       </c>
       <c r="D4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3570,10 +3571,10 @@
         <v>0.71875</v>
       </c>
       <c r="D5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3587,10 +3588,10 @@
         <v>0.78125</v>
       </c>
       <c r="D6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3604,10 +3605,10 @@
         <v>0.84375</v>
       </c>
       <c r="D7" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E7" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3626,7 +3627,7 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D9" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E9" t="s">
         <v>61</v>
@@ -3643,10 +3644,10 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3660,10 +3661,10 @@
         <v>0.71875</v>
       </c>
       <c r="D11" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E11" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3677,10 +3678,10 @@
         <v>0.78125</v>
       </c>
       <c r="D12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3694,10 +3695,10 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="D13" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E13" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3715,10 +3716,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D15" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E15" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3732,10 +3733,10 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E16" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3749,10 +3750,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D17" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3766,10 +3767,10 @@
         <v>0.71875</v>
       </c>
       <c r="D18" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E18" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3783,10 +3784,10 @@
         <v>0.78125</v>
       </c>
       <c r="D19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E19" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3800,10 +3801,10 @@
         <v>0.84375</v>
       </c>
       <c r="D20" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E20" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3821,7 +3822,7 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D22" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E22" t="s">
         <v>61</v>
@@ -3838,10 +3839,10 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D23" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E23" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3855,10 +3856,10 @@
         <v>0.71875</v>
       </c>
       <c r="D24" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E24" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3872,10 +3873,10 @@
         <v>0.78125</v>
       </c>
       <c r="D25" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E25" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3889,7 +3890,7 @@
         <v>0.84375</v>
       </c>
       <c r="D26" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="E26" t="s">
         <v>112</v>
@@ -3910,10 +3911,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D28" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E28" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3927,10 +3928,10 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D29" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E29" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3944,10 +3945,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D30" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E30" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -3961,10 +3962,10 @@
         <v>0.71875</v>
       </c>
       <c r="D31" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E31" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3978,10 +3979,10 @@
         <v>0.78125</v>
       </c>
       <c r="D32" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E32" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3995,10 +3996,10 @@
         <v>0.84375</v>
       </c>
       <c r="D33" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E33" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -4016,10 +4017,10 @@
         <v>0.38541666666666669</v>
       </c>
       <c r="D35" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E35" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -4033,10 +4034,10 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D36" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E36" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -4050,10 +4051,10 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="D37" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E37" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -4071,7 +4072,7 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D39" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E39" t="s">
         <v>61</v>
@@ -4088,7 +4089,7 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="D40" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E40" t="s">
         <v>61</v>
@@ -4105,10 +4106,10 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="D41" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E41" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -4160,7 +4161,7 @@
         <v>0.375</v>
       </c>
       <c r="D2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E2" t="s">
         <v>73</v>
@@ -4194,10 +4195,10 @@
         <v>0.5625</v>
       </c>
       <c r="D4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E4" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4211,7 +4212,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E5" t="s">
         <v>191</v>
@@ -4228,7 +4229,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D6" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E6" t="s">
         <v>74</v>
@@ -4263,10 +4264,10 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>372</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1">
@@ -4280,7 +4281,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>74</v>
@@ -4297,7 +4298,7 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>94</v>
@@ -4314,10 +4315,10 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>348</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1">
@@ -4331,7 +4332,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>210</v>
@@ -4348,7 +4349,7 @@
         <v>0.4375</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>210</v>
@@ -4365,7 +4366,7 @@
         <v>0.375</v>
       </c>
       <c r="D16" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>27</v>
@@ -4382,7 +4383,7 @@
         <v>0.4375</v>
       </c>
       <c r="D17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>207</v>
@@ -4399,7 +4400,7 @@
         <v>0.5</v>
       </c>
       <c r="D18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>208</v>
@@ -4416,7 +4417,7 @@
         <v>0.5625</v>
       </c>
       <c r="D19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>210</v>
@@ -4433,7 +4434,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D20" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E20" s="32" t="s">
         <v>206</v>
@@ -4450,7 +4451,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D21" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>32</v>
@@ -4467,7 +4468,7 @@
         <v>0.84375</v>
       </c>
       <c r="D22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>72</v>
@@ -4518,7 +4519,7 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="D26" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>74</v>
@@ -4535,7 +4536,7 @@
         <v>0.57291666666666663</v>
       </c>
       <c r="D27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>210</v>
@@ -4552,10 +4553,10 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D28" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -4569,7 +4570,7 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="D29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E29" s="32" t="s">
         <v>213</v>
@@ -4586,7 +4587,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D31" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>211</v>
@@ -4603,7 +4604,7 @@
         <v>0.5</v>
       </c>
       <c r="D32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>51</v>
@@ -4620,7 +4621,7 @@
         <v>0.57291666666666663</v>
       </c>
       <c r="D33" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>212</v>
@@ -4637,7 +4638,7 @@
         <v>0.4375</v>
       </c>
       <c r="D35" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>207</v>
@@ -4654,7 +4655,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="D36" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>213</v>
@@ -4671,7 +4672,7 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D38" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>246</v>
@@ -4688,7 +4689,7 @@
         <v>0.71875</v>
       </c>
       <c r="D39" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E39" s="32" t="s">
         <v>209</v>
@@ -4732,7 +4733,7 @@
         <v>44</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4746,13 +4747,13 @@
         <v>0.4375</v>
       </c>
       <c r="D2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4766,7 +4767,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -4783,7 +4784,7 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -4800,7 +4801,7 @@
         <v>0.8125</v>
       </c>
       <c r="D6" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
@@ -4817,10 +4818,10 @@
         <v>0.4375</v>
       </c>
       <c r="D8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4834,7 +4835,7 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -4851,10 +4852,10 @@
         <v>0.8125</v>
       </c>
       <c r="D11" t="s">
+        <v>321</v>
+      </c>
+      <c r="E11" t="s">
         <v>322</v>
-      </c>
-      <c r="E11" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4868,10 +4869,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4885,10 +4886,10 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="D14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4906,10 +4907,10 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="D16" t="s">
+        <v>321</v>
+      </c>
+      <c r="E16" t="s">
         <v>322</v>
-      </c>
-      <c r="E16" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -4923,10 +4924,10 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D18" t="s">
+        <v>324</v>
+      </c>
+      <c r="E18" t="s">
         <v>325</v>
-      </c>
-      <c r="E18" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4940,10 +4941,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -4960,7 +4961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -4998,13 +4999,13 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="D2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E2" t="s">
         <v>296</v>
       </c>
-      <c r="E2" t="s">
-        <v>297</v>
-      </c>
       <c r="G2" s="30" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
@@ -5020,13 +5021,13 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E3" t="s">
         <v>298</v>
       </c>
-      <c r="E3" t="s">
-        <v>299</v>
-      </c>
       <c r="G3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -5040,10 +5041,10 @@
         <v>0.84375</v>
       </c>
       <c r="D4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -5057,7 +5058,7 @@
         <v>0.40625</v>
       </c>
       <c r="D6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E6" t="s">
         <v>177</v>
@@ -5074,10 +5075,10 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="D7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -5091,10 +5092,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D8" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -5108,10 +5109,10 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="D9" t="s">
+        <v>302</v>
+      </c>
+      <c r="E9" t="s">
         <v>303</v>
-      </c>
-      <c r="E9" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -5125,10 +5126,10 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="D11" t="s">
+        <v>304</v>
+      </c>
+      <c r="E11" t="s">
         <v>305</v>
-      </c>
-      <c r="E11" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -5142,10 +5143,10 @@
         <v>0.625</v>
       </c>
       <c r="D12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -5159,10 +5160,10 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="D13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -5176,10 +5177,10 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -5193,10 +5194,10 @@
         <v>0.6875</v>
       </c>
       <c r="D16" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5210,10 +5211,10 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="D17" t="s">
+        <v>302</v>
+      </c>
+      <c r="E17" t="s">
         <v>303</v>
-      </c>
-      <c r="E17" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5227,10 +5228,10 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="D19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5244,10 +5245,10 @@
         <v>0.625</v>
       </c>
       <c r="D20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5261,10 +5262,10 @@
         <v>0.84375</v>
       </c>
       <c r="D21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -5278,10 +5279,10 @@
         <v>0.40625</v>
       </c>
       <c r="D23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E23" t="s">
         <v>311</v>
-      </c>
-      <c r="E23" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5295,10 +5296,10 @@
         <v>0.5</v>
       </c>
       <c r="D24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -5312,10 +5313,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D25" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -5329,10 +5330,10 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D27" t="s">
+        <v>313</v>
+      </c>
+      <c r="E27" t="s">
         <v>314</v>
-      </c>
-      <c r="E27" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5346,10 +5347,10 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -5494,7 +5495,7 @@
         <v>219</v>
       </c>
       <c r="E7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5755,7 +5756,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>17</v>
@@ -5773,7 +5774,7 @@
         <v>0.71875</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>32</v>
@@ -5809,7 +5810,7 @@
         <v>0.8125</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>168</v>
@@ -5848,7 +5849,7 @@
         <v>38</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F28" s="29"/>
     </row>
@@ -5937,7 +5938,7 @@
         <v>218</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F34" s="29"/>
     </row>
@@ -5952,7 +5953,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D35" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E35" s="32" t="s">
         <v>37</v>
@@ -6297,7 +6298,7 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="D55" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>166</v>
@@ -6336,7 +6337,7 @@
         <v>223</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F57" s="29"/>
     </row>
@@ -6394,10 +6395,10 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D62" t="s">
+        <v>396</v>
+      </c>
+      <c r="E62" s="8" t="s">
         <v>397</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>398</v>
       </c>
       <c r="F62" s="31"/>
     </row>
@@ -6430,7 +6431,7 @@
         <v>0.5625</v>
       </c>
       <c r="D64" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>190</v>
@@ -6448,7 +6449,7 @@
         <v>0.64930555555555558</v>
       </c>
       <c r="D65" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>191</v>
@@ -6554,7 +6555,7 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D72" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>32</v>
@@ -6626,7 +6627,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D76" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E76" s="32" t="s">
         <v>167</v>
@@ -6797,7 +6798,7 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="D2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E2" t="s">
         <v>165</v>
@@ -6816,10 +6817,10 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="D3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="15"/>
@@ -6838,10 +6839,10 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="D4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
@@ -6860,10 +6861,10 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="15"/>
@@ -6882,10 +6883,10 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="D6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="15"/>
@@ -6904,7 +6905,7 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E7" t="s">
         <v>165</v>
@@ -7485,7 +7486,7 @@
         <v>98</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1">
@@ -7788,10 +7789,10 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D42" t="s">
+        <v>389</v>
+      </c>
+      <c r="E42" t="s">
         <v>390</v>
-      </c>
-      <c r="E42" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -7825,7 +7826,7 @@
         <v>98</v>
       </c>
       <c r="E44" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -7839,7 +7840,7 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="D45" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E45" t="s">
         <v>85</v>
@@ -7859,7 +7860,7 @@
         <v>113</v>
       </c>
       <c r="E47" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -7992,10 +7993,10 @@
         <v>0.36458333333333331</v>
       </c>
       <c r="D56" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E56" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -8148,7 +8149,7 @@
         <v>126</v>
       </c>
       <c r="E66" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -8196,10 +8197,10 @@
         <v>0.78125</v>
       </c>
       <c r="D69" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E69" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -8268,10 +8269,10 @@
         <v>0.40625</v>
       </c>
       <c r="D2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E2" t="s">
         <v>411</v>
-      </c>
-      <c r="E2" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -8285,10 +8286,10 @@
         <v>0.46875</v>
       </c>
       <c r="D3" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E3" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -8302,10 +8303,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8319,7 +8320,7 @@
         <v>0.625</v>
       </c>
       <c r="D5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E5" t="s">
         <v>109</v>
@@ -8336,10 +8337,10 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="D6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -8353,10 +8354,10 @@
         <v>0.78125</v>
       </c>
       <c r="D7" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -8370,10 +8371,10 @@
         <v>0.84375</v>
       </c>
       <c r="D8" t="s">
+        <v>413</v>
+      </c>
+      <c r="E8" t="s">
         <v>414</v>
-      </c>
-      <c r="E8" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1"/>
@@ -8388,10 +8389,10 @@
         <v>0.40625</v>
       </c>
       <c r="D10" t="s">
+        <v>415</v>
+      </c>
+      <c r="E10" t="s">
         <v>416</v>
-      </c>
-      <c r="E10" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1">
@@ -8405,10 +8406,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D11" t="s">
+        <v>417</v>
+      </c>
+      <c r="E11" t="s">
         <v>418</v>
-      </c>
-      <c r="E11" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1">
@@ -8422,7 +8423,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E12" t="s">
         <v>111</v>
@@ -8439,7 +8440,7 @@
         <v>0.63541666666666663</v>
       </c>
       <c r="D13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E13" t="s">
         <v>51</v>
@@ -8456,10 +8457,10 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1">
@@ -8473,7 +8474,7 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="D15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E15" t="s">
         <v>48</v>
@@ -8490,10 +8491,10 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="D16" t="s">
+        <v>422</v>
+      </c>
+      <c r="E16" t="s">
         <v>423</v>
-      </c>
-      <c r="E16" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -8507,10 +8508,10 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D18" t="s">
+        <v>424</v>
+      </c>
+      <c r="E18" t="s">
         <v>425</v>
-      </c>
-      <c r="E18" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -8524,10 +8525,10 @@
         <v>0.5</v>
       </c>
       <c r="D19" t="s">
+        <v>426</v>
+      </c>
+      <c r="E19" t="s">
         <v>427</v>
-      </c>
-      <c r="E19" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -8541,10 +8542,10 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D20" t="s">
+        <v>428</v>
+      </c>
+      <c r="E20" t="s">
         <v>429</v>
-      </c>
-      <c r="E20" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -8558,10 +8559,10 @@
         <v>0.63541666666666663</v>
       </c>
       <c r="D21" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E21" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -8575,10 +8576,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D22" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E22" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -8592,7 +8593,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D23" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E23" t="s">
         <v>121</v>
@@ -8609,10 +8610,10 @@
         <v>0.84375</v>
       </c>
       <c r="D24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E24" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -8626,10 +8627,10 @@
         <v>0.40625</v>
       </c>
       <c r="D26" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E26" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -8643,7 +8644,7 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D27" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E27" t="s">
         <v>83</v>
@@ -8660,10 +8661,10 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D28" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -8677,10 +8678,10 @@
         <v>0.625</v>
       </c>
       <c r="D29" t="s">
+        <v>434</v>
+      </c>
+      <c r="E29" t="s">
         <v>435</v>
-      </c>
-      <c r="E29" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -8694,10 +8695,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D30" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E30" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -8711,10 +8712,10 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="D31" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E31" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -8728,10 +8729,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D32" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E32" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -8745,10 +8746,10 @@
         <v>0.36458333333333331</v>
       </c>
       <c r="D34" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E34" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -8762,7 +8763,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D35" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E35" t="s">
         <v>83</v>
@@ -8779,10 +8780,10 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="D36" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -8796,10 +8797,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D37" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E37" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -8813,10 +8814,10 @@
         <v>0.625</v>
       </c>
       <c r="D38" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -8830,7 +8831,7 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="D40" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E40" t="s">
         <v>121</v>
@@ -8847,7 +8848,7 @@
         <v>0.8125</v>
       </c>
       <c r="D41" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E41" t="s">
         <v>95</v>
@@ -8864,10 +8865,10 @@
         <v>0.86458333333333337</v>
       </c>
       <c r="D42" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -8919,7 +8920,7 @@
         <v>0.84375</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E2" t="s">
         <v>141</v>
@@ -8936,7 +8937,7 @@
         <v>0.4375</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E3" t="s">
         <v>141</v>
@@ -8953,7 +8954,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E4" t="s">
         <v>141</v>
@@ -9010,10 +9011,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75">
@@ -9027,10 +9028,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75">
@@ -9049,10 +9050,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75">
@@ -9066,10 +9067,10 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="D6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75">
@@ -9088,10 +9089,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75">
@@ -9105,10 +9106,10 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="D9" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75">
@@ -9127,10 +9128,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D11" t="s">
+        <v>290</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>291</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75">
@@ -9147,7 +9148,7 @@
         <v>104</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75">
@@ -9166,10 +9167,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75">
@@ -9244,10 +9245,10 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="D2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" t="s">
         <v>274</v>
-      </c>
-      <c r="E2" t="s">
-        <v>275</v>
       </c>
       <c r="H2"/>
       <c r="I2"/>
@@ -9263,10 +9264,10 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G3" s="35"/>
       <c r="H3" s="35"/>
@@ -9284,10 +9285,10 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
@@ -9305,10 +9306,10 @@
         <v>0.78125</v>
       </c>
       <c r="D5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -9334,10 +9335,10 @@
         <v>0.3125</v>
       </c>
       <c r="D7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="28"/>
@@ -9355,10 +9356,10 @@
         <v>0.46875</v>
       </c>
       <c r="D8" t="s">
+        <v>278</v>
+      </c>
+      <c r="E8" t="s">
         <v>279</v>
-      </c>
-      <c r="E8" t="s">
-        <v>280</v>
       </c>
       <c r="G8" s="26"/>
       <c r="H8" s="28"/>
@@ -9376,10 +9377,10 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G9" s="35"/>
       <c r="H9" s="35"/>
@@ -9397,10 +9398,10 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="D10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G10" s="26"/>
       <c r="H10" s="28"/>
@@ -9426,10 +9427,10 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="D12" t="s">
+        <v>273</v>
+      </c>
+      <c r="E12" t="s">
         <v>274</v>
-      </c>
-      <c r="E12" t="s">
-        <v>275</v>
       </c>
       <c r="G12" s="26"/>
       <c r="H12" s="28"/>
@@ -9447,10 +9448,10 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="28"/>
@@ -9468,10 +9469,10 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D14" t="s">
+        <v>276</v>
+      </c>
+      <c r="E14" t="s">
         <v>277</v>
-      </c>
-      <c r="E14" t="s">
-        <v>278</v>
       </c>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
@@ -9489,10 +9490,10 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G15" s="26"/>
       <c r="H15" s="28"/>
@@ -9518,10 +9519,10 @@
         <v>0.3125</v>
       </c>
       <c r="D17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="28"/>
@@ -9539,10 +9540,10 @@
         <v>0.46875</v>
       </c>
       <c r="D18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G18" s="26"/>
       <c r="H18" s="28"/>
@@ -9560,10 +9561,10 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
@@ -9581,10 +9582,10 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="D20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G20" s="26"/>
       <c r="H20" s="28"/>
@@ -9610,10 +9611,10 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="D22" t="s">
+        <v>273</v>
+      </c>
+      <c r="E22" t="s">
         <v>274</v>
-      </c>
-      <c r="E22" t="s">
-        <v>275</v>
       </c>
       <c r="G22" s="26"/>
       <c r="H22" s="28"/>
@@ -9631,7 +9632,7 @@
         <v>0.44791666666666669</v>
       </c>
       <c r="D23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E23" t="s">
         <v>165</v>
@@ -9652,10 +9653,10 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="D24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G24" s="26"/>
       <c r="H24" s="28"/>
@@ -9673,10 +9674,10 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D25" t="s">
+        <v>273</v>
+      </c>
+      <c r="E25" t="s">
         <v>274</v>
-      </c>
-      <c r="E25" t="s">
-        <v>275</v>
       </c>
       <c r="G25" s="26"/>
       <c r="H25" s="28"/>
@@ -9702,10 +9703,10 @@
         <v>0.46875</v>
       </c>
       <c r="D27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G27" s="26"/>
       <c r="H27" s="28"/>
@@ -9723,10 +9724,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E28" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G28" s="26"/>
       <c r="H28" s="28"/>
@@ -9752,10 +9753,10 @@
         <v>0.46875</v>
       </c>
       <c r="D30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G30" s="26"/>
       <c r="H30" s="28"/>
@@ -9773,10 +9774,10 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G31" s="35"/>
       <c r="H31" s="35"/>
@@ -9868,7 +9869,7 @@
         <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -9882,10 +9883,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -9899,10 +9900,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -9916,10 +9917,10 @@
         <v>0.5625</v>
       </c>
       <c r="D4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" t="s">
         <v>264</v>
-      </c>
-      <c r="E4" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -9933,10 +9934,10 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -9950,10 +9951,10 @@
         <v>0.75</v>
       </c>
       <c r="D6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6" t="s">
         <v>264</v>
-      </c>
-      <c r="E6" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -9967,10 +9968,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -9984,10 +9985,10 @@
         <v>0.32291666666666669</v>
       </c>
       <c r="D8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -10001,10 +10002,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -10018,10 +10019,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E10" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -10035,10 +10036,10 @@
         <v>0.75</v>
       </c>
       <c r="D11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -10052,10 +10053,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -10069,10 +10070,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -10086,10 +10087,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -10103,10 +10104,10 @@
         <v>0.5625</v>
       </c>
       <c r="D15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -10120,10 +10121,10 @@
         <v>0.75</v>
       </c>
       <c r="D16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -10137,10 +10138,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -10154,10 +10155,10 @@
         <v>0.32291666666666669</v>
       </c>
       <c r="D18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -10171,10 +10172,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -10188,10 +10189,10 @@
         <v>0.75</v>
       </c>
       <c r="D20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -10205,10 +10206,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -10222,10 +10223,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -10239,10 +10240,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -10256,10 +10257,10 @@
         <v>0.5625</v>
       </c>
       <c r="D24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -10273,10 +10274,10 @@
         <v>0.75</v>
       </c>
       <c r="D25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -10290,10 +10291,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D26" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -10307,10 +10308,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -10324,10 +10325,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -10341,10 +10342,10 @@
         <v>0.5625</v>
       </c>
       <c r="D29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E29" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -10358,10 +10359,10 @@
         <v>0.75</v>
       </c>
       <c r="D30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -10375,10 +10376,10 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -10392,10 +10393,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -10409,10 +10410,10 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="D33" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -10426,10 +10427,10 @@
         <v>0.75</v>
       </c>
       <c r="D34" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>